<commit_message>
Started editing sulfide code for COMPASS May 2025 data
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/2025May_H2S_Datasheets.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/2025May_H2S_Datasheets.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GlobalChangeEco\Porewater_R scripts &amp; Data\Data\Sulfide Microplate\COMPASS\2025 May\Datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/May/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{92021526-6563-4582-BD6D-EF31E3B89D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE1C3B6F-C5F3-480F-82BF-09ABCF781D0A}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="2175" windowWidth="16815" windowHeight="11025" firstSheet="3" activeTab="9" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{23FB6DB2-3641-4E78-A68E-113D11F8B05A}"/>
   </bookViews>
   <sheets>
     <sheet name="STD" sheetId="1" r:id="rId1"/>
     <sheet name="Plate 1" sheetId="3" r:id="rId2"/>
     <sheet name="Plate 2" sheetId="4" r:id="rId3"/>
-    <sheet name="Plate 3" sheetId="5" r:id="rId4"/>
-    <sheet name="Plate 4" sheetId="6" r:id="rId5"/>
+    <sheet name="Plate 4" sheetId="6" r:id="rId4"/>
+    <sheet name="Plate 3" sheetId="5" r:id="rId5"/>
     <sheet name="Plate 5" sheetId="7" r:id="rId6"/>
     <sheet name="Plate 6" sheetId="8" r:id="rId7"/>
     <sheet name="Plate 7" sheetId="9" r:id="rId8"/>
@@ -662,9 +662,9 @@
       <selection activeCell="B18" sqref="B18:G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -703,7 +703,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -762,7 +762,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -822,7 +822,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -852,7 +852,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -882,7 +882,7 @@
       <c r="M7" s="4"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -912,7 +912,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -942,10 +942,10 @@
       <c r="M9" s="4"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -984,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1013,7 @@
       <c r="L12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1042,7 +1042,7 @@
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1100,7 +1100,7 @@
       <c r="L15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="L16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +1158,7 @@
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1187,7 +1187,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -1216,7 +1216,7 @@
       <c r="L19" s="4"/>
       <c r="M19" s="4"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -1232,17 +1232,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74720A33-EA02-4F3B-99BC-21807D7702E9}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1279,9 +1279,9 @@
       <selection activeCell="D12" sqref="D12:M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -1320,7 +1320,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1487,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1571,7 +1571,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -1613,7 +1613,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -1655,10 +1655,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -1697,7 +1697,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -2045,9 +2045,9 @@
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -2086,7 +2086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2211,7 +2211,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -2295,7 +2295,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2337,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -2421,10 +2421,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -2463,7 +2463,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -2627,7 +2627,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -2804,16 +2804,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22A4539-D444-41BA-86FA-1F5D324B909E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175D917F-D120-4FE6-B8A3-DF191DABB500}">
   <dimension ref="A1:N22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -2852,7 +2852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2866,34 +2866,34 @@
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="F2" s="5">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G2" s="5">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="H2" s="5">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="I2" s="5">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="J2" s="5">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="K2" s="5">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="L2" s="5">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="M2" s="5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2907,13 +2907,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="F3" s="5">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="G3" s="5">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>19</v>
@@ -2925,17 +2925,17 @@
         <v>19</v>
       </c>
       <c r="K3" s="5">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L3" s="5">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="M3" s="5">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -2949,35 +2949,35 @@
         <v>5</v>
       </c>
       <c r="E4" s="5">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="F4" s="5">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="G4" s="5">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="K4" s="5">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="L4" s="5">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="M4" s="5">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2991,13 +2991,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="5">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="F5" s="5">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G5" s="5">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>20</v>
@@ -3009,17 +3009,15 @@
         <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>38</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="L5" s="5"/>
       <c r="M5" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3033,35 +3031,35 @@
         <v>9</v>
       </c>
       <c r="E6" s="5">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="F6" s="5">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="G6" s="5">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="H6" s="5">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="I6" s="5">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="J6" s="5">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3075,22 +3073,22 @@
         <v>11</v>
       </c>
       <c r="E7" s="5">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="F7" s="5">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="G7" s="5">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="H7" s="5">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="I7" s="5">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="J7" s="5">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>19</v>
@@ -3103,7 +3101,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3117,35 +3115,35 @@
         <v>13</v>
       </c>
       <c r="E8" s="5">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="F8" s="5">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="G8" s="5">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5">
+        <v>60</v>
+      </c>
+      <c r="I8" s="5">
+        <v>60</v>
+      </c>
+      <c r="J8" s="5">
+        <v>60</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="I8" s="5">
+      <c r="L8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="5">
+      <c r="M8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3159,22 +3157,22 @@
         <v>22</v>
       </c>
       <c r="E9" s="5">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="F9" s="5">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="G9" s="5">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="H9" s="5">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="I9" s="5">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="J9" s="5">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>21</v>
@@ -3187,10 +3185,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -3229,7 +3227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -3243,13 +3241,13 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="F12" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
@@ -3261,16 +3259,16 @@
         <v>1</v>
       </c>
       <c r="K12" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L12" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M12" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -3302,16 +3300,16 @@
         <v>1</v>
       </c>
       <c r="K13" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L13" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M13" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -3343,16 +3341,16 @@
         <v>1</v>
       </c>
       <c r="K14" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L14" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M14" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -3384,16 +3382,14 @@
         <v>1</v>
       </c>
       <c r="K15" s="4">
-        <v>1</v>
-      </c>
-      <c r="L15" s="4">
-        <v>1</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="L15" s="4"/>
       <c r="M15" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -3416,25 +3412,25 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I16" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K16" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L16" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M16" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -3457,13 +3453,13 @@
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I17" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J17" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K17" s="4">
         <v>1</v>
@@ -3475,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -3498,25 +3494,25 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I18" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J18" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K18" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L18" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="M18" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -3539,13 +3535,13 @@
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I19" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="J19" s="4">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="K19" s="4">
         <v>1</v>
@@ -3557,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -3570,16 +3566,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175D917F-D120-4FE6-B8A3-DF191DABB500}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F22A4539-D444-41BA-86FA-1F5D324B909E}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -3618,7 +3614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -3632,34 +3628,34 @@
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="F2" s="5">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="G2" s="5">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="H2" s="5">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="I2" s="5">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="J2" s="5">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="K2" s="5">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="L2" s="5">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="M2" s="5">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3673,13 +3669,13 @@
         <v>3</v>
       </c>
       <c r="E3" s="5">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="F3" s="5">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G3" s="5">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>19</v>
@@ -3691,17 +3687,17 @@
         <v>19</v>
       </c>
       <c r="K3" s="5">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="L3" s="5">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="M3" s="5">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -3715,35 +3711,35 @@
         <v>5</v>
       </c>
       <c r="E4" s="5">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="F4" s="5">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="G4" s="5">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="K4" s="5">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="L4" s="5">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="M4" s="5">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -3757,13 +3753,13 @@
         <v>7</v>
       </c>
       <c r="E5" s="5">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F5" s="5">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="G5" s="5">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>20</v>
@@ -3775,15 +3771,17 @@
         <v>20</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="M5" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -3797,35 +3795,35 @@
         <v>9</v>
       </c>
       <c r="E6" s="5">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="G6" s="5">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="H6" s="5">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="I6" s="5">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="J6" s="5">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -3839,22 +3837,22 @@
         <v>11</v>
       </c>
       <c r="E7" s="5">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="F7" s="5">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="G7" s="5">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="H7" s="5">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="I7" s="5">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="J7" s="5">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>19</v>
@@ -3867,7 +3865,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -3881,35 +3879,35 @@
         <v>13</v>
       </c>
       <c r="E8" s="5">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F8" s="5">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="G8" s="5">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="H8" s="5">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="I8" s="5">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="J8" s="5">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -3923,22 +3921,22 @@
         <v>22</v>
       </c>
       <c r="E9" s="5">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="F9" s="5">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="G9" s="5">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="H9" s="5">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="I9" s="5">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="J9" s="5">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>21</v>
@@ -3951,10 +3949,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -3993,7 +3991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -4007,34 +4005,34 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>1</v>
+      </c>
+      <c r="K12" s="4">
         <v>25</v>
       </c>
-      <c r="F12" s="4">
+      <c r="L12" s="4">
         <v>25</v>
       </c>
-      <c r="G12" s="4">
+      <c r="M12" s="4">
         <v>25</v>
       </c>
-      <c r="H12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4">
-        <v>1</v>
-      </c>
-      <c r="J12" s="4">
-        <v>1</v>
-      </c>
-      <c r="K12" s="4">
-        <v>1</v>
-      </c>
-      <c r="L12" s="4">
-        <v>1</v>
-      </c>
-      <c r="M12" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -4066,16 +4064,16 @@
         <v>1</v>
       </c>
       <c r="K13" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L13" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M13" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -4107,16 +4105,16 @@
         <v>1</v>
       </c>
       <c r="K14" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L14" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M14" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -4148,14 +4146,16 @@
         <v>1</v>
       </c>
       <c r="K15" s="4">
-        <v>25</v>
-      </c>
-      <c r="L15" s="4"/>
+        <v>1</v>
+      </c>
+      <c r="L15" s="4">
+        <v>1</v>
+      </c>
       <c r="M15" s="4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -4178,25 +4178,25 @@
         <v>1</v>
       </c>
       <c r="H16" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I16" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J16" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K16" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L16" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -4219,13 +4219,13 @@
         <v>1</v>
       </c>
       <c r="H17" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I17" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J17" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K17" s="4">
         <v>1</v>
@@ -4237,7 +4237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -4260,25 +4260,25 @@
         <v>1</v>
       </c>
       <c r="H18" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I18" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J18" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K18" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="L18" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="M18" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -4301,13 +4301,13 @@
         <v>1</v>
       </c>
       <c r="H19" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="I19" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="J19" s="4">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="K19" s="4">
         <v>1</v>
@@ -4319,7 +4319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -4339,9 +4339,9 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -4380,7 +4380,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4463,7 +4463,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -4547,7 +4547,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -4673,7 +4673,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -4715,10 +4715,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -4757,7 +4757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -5003,7 +5003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -5044,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -5085,7 +5085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -5105,9 +5105,9 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -5146,7 +5146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5187,7 +5187,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5229,7 +5229,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -5313,7 +5313,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -5355,7 +5355,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -5481,10 +5481,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -5523,7 +5523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -5687,7 +5687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -5728,7 +5728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -5810,7 +5810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -5871,9 +5871,9 @@
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -5912,7 +5912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5995,7 +5995,7 @@
       </c>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -6037,7 +6037,7 @@
       </c>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -6079,7 +6079,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -6161,7 +6161,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -6203,7 +6203,7 @@
       </c>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -6245,10 +6245,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -6287,7 +6287,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -6328,7 +6328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -6451,7 +6451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -6531,7 +6531,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -6613,7 +6613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>
@@ -6633,9 +6633,9 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -6674,7 +6674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -6709,7 +6709,7 @@
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -6745,7 +6745,7 @@
       <c r="M3" s="5"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -6781,7 +6781,7 @@
       <c r="M4" s="5"/>
       <c r="N4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -6823,7 +6823,7 @@
       </c>
       <c r="N5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -6907,7 +6907,7 @@
       </c>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -6943,7 +6943,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -6985,10 +6985,10 @@
       </c>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2">
         <v>1</v>
@@ -7027,7 +7027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -7068,7 +7068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -7109,7 +7109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -7273,7 +7273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>12</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -7355,7 +7355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>15</v>
       </c>

</xml_diff>